<commit_message>
day 28 write into Excel file
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lutic\IdeaProjects\Fall2019Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2249A36A-07F2-4294-B93A-CA992BC6B8A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DAFF91-A480-4FB0-B2B8-C9280643FB81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3914" uniqueCount="1481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1480">
   <si>
     <t>username</t>
   </si>
@@ -4475,17 +4475,13 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>Date of execution</t>
-  </si>
-  <si>
-    <t>2020-04-14T20:43:51.267881400</t>
+    <t>SKIPPED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4839,8 +4835,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -9083,8 +9079,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -9124,7 +9120,7 @@
         <v>305</v>
       </c>
       <c r="F2" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -9144,7 +9140,7 @@
         <v>803</v>
       </c>
       <c r="F3" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -9164,7 +9160,7 @@
         <v>805</v>
       </c>
       <c r="F4" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -9184,7 +9180,7 @@
         <v>460</v>
       </c>
       <c r="F5" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -9204,7 +9200,7 @@
         <v>439</v>
       </c>
       <c r="F6" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -9224,7 +9220,7 @@
         <v>501</v>
       </c>
       <c r="F7" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -9244,7 +9240,7 @@
         <v>935</v>
       </c>
       <c r="F8" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -9264,7 +9260,7 @@
         <v>937</v>
       </c>
       <c r="F9" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -9284,7 +9280,7 @@
         <v>939</v>
       </c>
       <c r="F10" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -9304,7 +9300,7 @@
         <v>603</v>
       </c>
       <c r="F11" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -9324,7 +9320,7 @@
         <v>1062</v>
       </c>
       <c r="F12" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -9344,7 +9340,7 @@
         <v>1064</v>
       </c>
       <c r="F13" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -9364,7 +9360,7 @@
         <v>1066</v>
       </c>
       <c r="F14" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -9384,7 +9380,7 @@
         <v>399</v>
       </c>
       <c r="F15" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -9404,7 +9400,7 @@
         <v>636</v>
       </c>
       <c r="F16" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
     </row>
   </sheetData>
@@ -9422,8 +9418,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -13669,8 +13665,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -14008,8 +14004,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -18247,16 +18243,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C30F00C-C683-0548-B7C4-02FB1EBCAEF1}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -18278,9 +18274,6 @@
       <c r="F1" t="s">
         <v>1476</v>
       </c>
-      <c r="G1" t="s">
-        <v>1479</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -18299,10 +18292,7 @@
         <v>305</v>
       </c>
       <c r="F2" t="s">
-        <v>1478</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>